<commit_message>
added checks for no description, invalid header
</commit_message>
<xml_diff>
--- a/tests/data/validate_tables/no_id.xlsx
+++ b/tests/data/validate_tables/no_id.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-data-tools/tests/data/validate_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5495252C-8FBF-5440-82B5-A5BF1181AE4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15739A3F-A223-924E-9B2D-F87371A75210}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="6220" windowWidth="23400" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3060" yWindow="2280" windowWidth="23400" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>variable</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>order</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -464,7 +467,7 @@
     <col min="8" max="8" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +504,11 @@
       <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -510,7 +516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>

</xml_diff>